<commit_message>
Add in eligibility criteria
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/eligibility_criteria_1.xlsx
+++ b/tests/integration_test_files/eligibility_criteria_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1624754B-50BA-CE4B-A33F-73F0B54D8020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D85777-5C97-954B-A6EF-F02BE4A3CECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="59860" yWindow="4900" windowWidth="33600" windowHeight="19480" firstSheet="1" activeTab="5" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="59860" yWindow="4900" windowWidth="33600" windowHeight="19480" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -1851,9 +1851,6 @@
     <t>country : GBR, country:FRA, region:ASIA, country :USA</t>
   </si>
   <si>
-    <t>region=asia</t>
-  </si>
-  <si>
     <t>identifier</t>
   </si>
   <si>
@@ -1924,6 +1921,9 @@
   </si>
   <si>
     <t>Population three, old age group</t>
+  </si>
+  <si>
+    <t>region:asia</t>
   </si>
 </sst>
 </file>
@@ -2414,8 +2414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53AA772F-4124-4842-BA10-D27E5C5CE960}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17:G19"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2629,7 +2629,7 @@
         <v>44958</v>
       </c>
       <c r="G19" t="s">
-        <v>589</v>
+        <v>613</v>
       </c>
     </row>
   </sheetData>
@@ -2829,10 +2829,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B2" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -2849,10 +2849,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B3" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C3">
         <v>20</v>
@@ -2869,10 +2869,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B4" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C4">
         <v>20</v>
@@ -5557,7 +5557,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ED1B92D-F8EC-D24D-81E6-6B85449D22F0}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -5576,7 +5576,7 @@
         <v>553</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="C1" s="22" t="s">
         <v>481</v>
@@ -5591,27 +5591,27 @@
         <v>284</v>
       </c>
       <c r="G1" s="22" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>603</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>604</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" t="s">
         <v>605</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>606</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>607</v>
       </c>
-      <c r="F2" t="s">
-        <v>608</v>
-      </c>
       <c r="G2" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
   </sheetData>
@@ -5647,36 +5647,36 @@
         <v>554</v>
       </c>
       <c r="D1" s="22" t="s">
+        <v>591</v>
+      </c>
+      <c r="E1" s="22" t="s">
         <v>592</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="F1" s="22" t="s">
         <v>593</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="G1" s="22" t="s">
         <v>594</v>
-      </c>
-      <c r="G1" s="22" t="s">
-        <v>595</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>595</v>
+      </c>
+      <c r="B2" t="s">
         <v>596</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>597</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>598</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>599</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>600</v>
-      </c>
-      <c r="F2" t="s">
-        <v>601</v>
       </c>
       <c r="G2" t="s">
         <v>74</v>
@@ -5684,16 +5684,16 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
+        <v>601</v>
+      </c>
+      <c r="E3" t="s">
+        <v>599</v>
+      </c>
+      <c r="F3" t="s">
+        <v>600</v>
+      </c>
+      <c r="G3" t="s">
         <v>602</v>
-      </c>
-      <c r="E3" t="s">
-        <v>600</v>
-      </c>
-      <c r="F3" t="s">
-        <v>601</v>
-      </c>
-      <c r="G3" t="s">
-        <v>603</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add further error checks and dictionary validation
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/eligibility_criteria_1.xlsx
+++ b/tests/integration_test_files/eligibility_criteria_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D85777-5C97-954B-A6EF-F02BE4A3CECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{890EE4C1-3D9B-2547-8E8E-6FCFB63A1329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="59860" yWindow="4900" windowWidth="33600" windowHeight="19480" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="59860" yWindow="4900" windowWidth="33600" windowHeight="19480" activeTab="5" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="614">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="618">
   <si>
     <t>Epoch</t>
   </si>
@@ -1924,6 +1924,18 @@
   </si>
   <si>
     <t>region:asia</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>Age Criteria Error</t>
+  </si>
+  <si>
+    <t>The study age criterion with error</t>
+  </si>
+  <si>
+    <t>Subjects shall be between [min_age] and [max_agexxx]</t>
   </si>
 </sst>
 </file>
@@ -2414,7 +2426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53AA772F-4124-4842-BA10-D27E5C5CE960}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -5555,9 +5567,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ED1B92D-F8EC-D24D-81E6-6B85449D22F0}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -5611,6 +5623,26 @@
         <v>607</v>
       </c>
       <c r="G2" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>603</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>614</v>
+      </c>
+      <c r="C3" t="s">
+        <v>615</v>
+      </c>
+      <c r="D3" t="s">
+        <v>616</v>
+      </c>
+      <c r="F3" t="s">
+        <v>617</v>
+      </c>
+      <c r="G3" t="s">
         <v>595</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix test file typo
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/eligibility_criteria_1.xlsx
+++ b/tests/integration_test_files/eligibility_criteria_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{890EE4C1-3D9B-2547-8E8E-6FCFB63A1329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D2A9C3-134E-8E47-B2DB-D8FE271304BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="59860" yWindow="4900" windowWidth="33600" windowHeight="19480" activeTab="5" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="36160" yWindow="5100" windowWidth="33600" windowHeight="19480" firstSheet="5" activeTab="6" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="618">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="617">
   <si>
     <t>Epoch</t>
   </si>
@@ -1888,9 +1888,6 @@
   </si>
   <si>
     <t>max_age</t>
-  </si>
-  <si>
-    <t>plannedMaxuímumAgeOfParticipants</t>
   </si>
   <si>
     <t>Inclusion</t>
@@ -2641,7 +2638,7 @@
         <v>44958</v>
       </c>
       <c r="G19" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
   </sheetData>
@@ -2844,7 +2841,7 @@
         <v>600</v>
       </c>
       <c r="B2" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -2861,10 +2858,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B3" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="C3">
         <v>20</v>
@@ -2881,10 +2878,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B4" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C4">
         <v>20</v>
@@ -5569,7 +5566,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ED1B92D-F8EC-D24D-81E6-6B85449D22F0}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -5608,19 +5605,19 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>602</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>603</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" t="s">
         <v>604</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>605</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>606</v>
-      </c>
-      <c r="F2" t="s">
-        <v>607</v>
       </c>
       <c r="G2" t="s">
         <v>595</v>
@@ -5628,19 +5625,19 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>613</v>
+      </c>
+      <c r="C3" t="s">
         <v>614</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>615</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>616</v>
-      </c>
-      <c r="F3" t="s">
-        <v>617</v>
       </c>
       <c r="G3" t="s">
         <v>595</v>
@@ -5655,8 +5652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EB40753-8F7D-3941-9F21-F336F33F75CC}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5725,7 +5722,7 @@
         <v>600</v>
       </c>
       <c r="G3" t="s">
-        <v>602</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix more XL files timeline sheets
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/eligibility_criteria_1.xlsx
+++ b/tests/integration_test_files/eligibility_criteria_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28067E0D-D255-904D-8977-89347AA59453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D077AE4E-C57E-054E-9115-3A2B2F8D92A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="53400" yWindow="5420" windowWidth="33600" windowHeight="19480" firstSheet="9" activeTab="14" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="53400" yWindow="5420" windowWidth="33600" windowHeight="19480" firstSheet="8" activeTab="8" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="680">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="680">
   <si>
     <t>Screening</t>
   </si>
@@ -2295,10 +2295,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3456,7 +3456,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B908C5D6-C6A1-4043-A49A-69C599CFBAE9}">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="E2" sqref="E2:E3"/>
     </sheetView>
   </sheetViews>
@@ -6034,34 +6034,34 @@
       <c r="A3" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
@@ -6181,16 +6181,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6517,11 +6517,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136502A0-3DDE-CC47-9DA7-EB2F3073B24B}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" sqref="A1:H1048576"/>
+      <selection pane="bottomRight" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6720,9 +6720,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="A10" s="2"/>
       <c r="B10" s="3" t="s">
         <v>5</v>
       </c>
@@ -6746,9 +6744,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="A11" s="2"/>
       <c r="B11" s="4" t="s">
         <v>12</v>
       </c>

</xml_diff>